<commit_message>
puse la pestaña tasa
</commit_message>
<xml_diff>
--- a/Bonos en pesos.xlsx
+++ b/Bonos en pesos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18615" windowHeight="7665" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18615" windowHeight="7665"/>
   </bookViews>
   <sheets>
     <sheet name="Flujo Cartera Escalera" sheetId="16" r:id="rId1"/>
@@ -44779,8 +44779,8 @@
   <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50361,7 +50361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -50765,7 +50765,7 @@
     <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29">
         <f ca="1">TODAY()</f>
-        <v>44489</v>
+        <v>44508</v>
       </c>
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
@@ -50776,7 +50776,7 @@
       <c r="F5" s="22"/>
       <c r="G5" s="32">
         <f ca="1">TODAY()</f>
-        <v>44489</v>
+        <v>44508</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
@@ -50852,7 +50852,7 @@
       </c>
       <c r="L7" s="20">
         <f ca="1">G8-G5</f>
-        <v>223</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -50889,7 +50889,7 @@
       </c>
       <c r="L8" s="20">
         <f ca="1">L7/30</f>
-        <v>7.4333333333333336</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -50911,7 +50911,7 @@
       </c>
       <c r="F9" s="22">
         <f ca="1">A11-A5</f>
-        <v>349</v>
+        <v>330</v>
       </c>
       <c r="G9" s="34"/>
       <c r="H9" s="28">
@@ -50948,7 +50948,7 @@
       </c>
       <c r="F10" s="22">
         <f ca="1">F9/30</f>
-        <v>11.633333333333333</v>
+        <v>11</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="23"/>
@@ -50957,7 +50957,7 @@
       </c>
       <c r="J10" s="51">
         <f ca="1">XIRR(J5:J8,G5:G8)</f>
-        <v>0.4417095005512236</v>
+        <v>0.49783237576484674</v>
       </c>
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
@@ -51022,9 +51022,9 @@
       <c r="C13" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="51" t="e">
         <f ca="1">XIRR(D5:D11,A5:A11)</f>
-        <v>4.2356688261032112</v>
+        <v>#NUM!</v>
       </c>
       <c r="E13" s="28"/>
       <c r="F13" s="22"/>
@@ -51034,7 +51034,7 @@
       </c>
       <c r="J13" s="66">
         <f ca="1">J12/L8</f>
-        <v>3.0279667028968995</v>
+        <v>3.3099832095392578</v>
       </c>
       <c r="Q13" s="22"/>
     </row>
@@ -51078,7 +51078,7 @@
       </c>
       <c r="D16" s="28">
         <f ca="1">D15/F10</f>
-        <v>3.1908309455587394</v>
+        <v>3.3745454545454545</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="44" t="s">
@@ -51103,7 +51103,7 @@
       <c r="F17" s="22"/>
       <c r="G17" s="50">
         <f ca="1">TODAY()</f>
-        <v>44489</v>
+        <v>44508</v>
       </c>
       <c r="H17" s="59"/>
       <c r="I17" s="57"/>
@@ -51151,7 +51151,7 @@
       </c>
       <c r="N18" s="50">
         <f ca="1">TODAY()</f>
-        <v>44489</v>
+        <v>44508</v>
       </c>
       <c r="O18" s="75"/>
       <c r="P18" s="75"/>
@@ -51162,7 +51162,7 @@
     <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24">
         <f ca="1">TODAY()</f>
-        <v>44489</v>
+        <v>44508</v>
       </c>
       <c r="B19" s="49"/>
       <c r="C19" s="48"/>
@@ -51343,7 +51343,7 @@
       </c>
       <c r="L23">
         <f ca="1">G22-G17</f>
-        <v>727</v>
+        <v>708</v>
       </c>
       <c r="N23" s="35">
         <v>44838</v>
@@ -51362,7 +51362,7 @@
       </c>
       <c r="S23">
         <f ca="1">N23-N18</f>
-        <v>349</v>
+        <v>330</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -51387,7 +51387,7 @@
       </c>
       <c r="L24" s="1">
         <f ca="1">L23/30</f>
-        <v>24.233333333333334</v>
+        <v>23.6</v>
       </c>
       <c r="O24" s="16">
         <f>SUM(O19:O23)</f>
@@ -51406,7 +51406,7 @@
       </c>
       <c r="S24">
         <f ca="1">S23/30</f>
-        <v>11.633333333333333</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -51429,7 +51429,7 @@
       </c>
       <c r="J25" s="62">
         <f ca="1">XIRR(J17:J22,G17:G22)</f>
-        <v>0.57155789732933071</v>
+        <v>0.59727287888526914</v>
       </c>
       <c r="S25" s="22"/>
     </row>
@@ -51460,7 +51460,7 @@
       </c>
       <c r="Q26" s="62">
         <f ca="1">XIRR(Q18:Q23,N18:N23)</f>
-        <v>0.76365395784378065</v>
+        <v>0.91950997114181532</v>
       </c>
       <c r="S26" s="22"/>
     </row>
@@ -51515,7 +51515,7 @@
       </c>
       <c r="J28" s="66">
         <f ca="1">J27/L24</f>
-        <v>4.4322176371694937</v>
+        <v>4.5511613308223478</v>
       </c>
       <c r="P28" s="66" t="s">
         <v>37</v>
@@ -51548,7 +51548,7 @@
       </c>
       <c r="Q29">
         <f ca="1">Q28/S24</f>
-        <v>2.4723288461191908</v>
+        <v>2.6146750524109019</v>
       </c>
       <c r="S29" s="22"/>
     </row>
@@ -51644,7 +51644,7 @@
       </c>
       <c r="F34">
         <f ca="1">A35-A19</f>
-        <v>1270</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="35" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -51665,7 +51665,7 @@
       </c>
       <c r="F35" s="1">
         <f ca="1">F34/30</f>
-        <v>42.333333333333336</v>
+        <v>41.7</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
@@ -51688,7 +51688,7 @@
       </c>
       <c r="D38" s="62">
         <f ca="1">XIRR(D19:D35,A19:A35)</f>
-        <v>0.82772961854934679</v>
+        <v>0.87738255262374865</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -51715,7 +51715,7 @@
       </c>
       <c r="D41">
         <f ca="1">D40/F35</f>
-        <v>4.6340870773506246</v>
+        <v>4.704468895471857</v>
       </c>
       <c r="F41" s="39"/>
       <c r="T41" s="22"/>
@@ -51785,7 +51785,7 @@
       </c>
       <c r="D51" s="51">
         <f ca="1">XIRR(J17:J22,G17:G22)</f>
-        <v>0.57155789732933071</v>
+        <v>0.59727287888526914</v>
       </c>
       <c r="T51" s="22"/>
       <c r="U51" s="28"/>

</xml_diff>